<commit_message>
Added size classes from Fishbase
</commit_message>
<xml_diff>
--- a/Data/Raw/Ashmore_BRUV_naming_key.xlsx
+++ b/Data/Raw/Ashmore_BRUV_naming_key.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6eb6a0b2b1d48aff/Documents/Repositories/Ashmore_BRUVS/Data/Raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{00436A59-D380-4B2C-A2FC-351FF29A980C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{00436A59-D380-4B2C-A2FC-351FF29A980C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34AE8CF9-4E83-41B8-A219-1BC9A52E9C6E}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{E683A478-F546-C441-8626-E7E9BD84878B}"/>
+    <workbookView minimized="1" xWindow="2380" yWindow="3090" windowWidth="11070" windowHeight="8170" activeTab="1" xr2:uid="{E683A478-F546-C441-8626-E7E9BD84878B}"/>
   </bookViews>
   <sheets>
     <sheet name="vid names final subsample" sheetId="1" r:id="rId1"/>
@@ -1125,7 +1125,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{906D0127-D583-B241-BCF9-4E0A2EB840E1}">
   <dimension ref="A1:B49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A27" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -1537,14 +1537,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8DD9F2C-1A7C-4EA8-98FF-0DF93B38DF22}">
   <dimension ref="A1:J222"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F205" sqref="F205:I205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="18.9140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">

</xml_diff>